<commit_message>
half done with admin side started voter side
</commit_message>
<xml_diff>
--- a/src/excels/testsheet.xlsx
+++ b/src/excels/testsheet.xlsx
@@ -20,27 +20,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t xml:space="preserve">No</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t xml:space="preserve">studentid</t>
   </si>
   <si>
     <t xml:space="preserve">name</t>
   </si>
   <si>
-    <t xml:space="preserve">id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sammy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">christy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">joel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emmma</t>
+    <t xml:space="preserve">secrettoken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kassim Balogun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">er2345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Richard Alipui</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tf4534</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Papa Kofi Gyekye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2hg432</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peter Perez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6ty435</t>
   </si>
 </sst>
 </file>
@@ -55,6 +67,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -138,13 +151,16 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="156" zoomScaleNormal="156" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -160,46 +176,46 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1</v>
+        <v>34010231</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>2345</v>
+      <c r="C2" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>2</v>
+        <v>34562212</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>4534</v>
+        <v>5</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>3</v>
+        <v>34516066</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>2432</v>
+        <v>7</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>4</v>
+        <v>34917894</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>6435</v>
+        <v>9</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>